<commit_message>
BB-21840: Remove import results dialog (#34030)
- added QuickAddController::importOptimizedAction
- added QuickAddImportResultsProvider and basic provider for formatting QuickAddCollection for usage on storefornt
- added QuickAddCollectionPriceProvider::addAllPrices to return all prices for optimized quick add form
- added switch for optimized form to CalculatePriceForCollectionListener
- added switch for optimized form routes to ProductFormProvider
- changed QuickAddRowInputParser so it returns unit even if it is unresolved
- added ability to specify property path in QuickAddRow::addError
- added tests
</commit_message>
<xml_diff>
--- a/src/Oro/Bundle/ProductBundle/Tests/Functional/Controller/Frontend/files/quick-order.xlsx
+++ b/src/Oro/Bundle/ProductBundle/Tests/Functional/Controller/Frontend/files/quick-order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">product-1</t>
   </si>
   <si>
-    <t xml:space="preserve">1,4</t>
+    <t xml:space="preserve">1.4</t>
   </si>
   <si>
     <t xml:space="preserve">liter</t>
@@ -69,7 +69,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -97,12 +97,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -173,53 +167,53 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z65536"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -550,7 +544,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
BB-21840: Remove import results dialog (#34032)
- added QuickAddController::importOptimizedAction
- added QuickAddImportResultsProvider and basic provider for formatting QuickAddCollection for usage on storefornt
- added QuickAddCollectionPriceProvider::addAllPrices to return all prices for optimized quick add form
- added switch for optimized form to CalculatePriceForCollectionListener
- added switch for optimized form routes to ProductFormProvider
- changed QuickAddRowInputParser so it returns unit even if it is unresolved
- added ability to specify property path in QuickAddRow::addError
- added tests
</commit_message>
<xml_diff>
--- a/src/Oro/Bundle/ProductBundle/Tests/Functional/Controller/Frontend/files/quick-order.xlsx
+++ b/src/Oro/Bundle/ProductBundle/Tests/Functional/Controller/Frontend/files/quick-order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">product-1</t>
   </si>
   <si>
-    <t xml:space="preserve">1,4</t>
+    <t xml:space="preserve">1.4</t>
   </si>
   <si>
     <t xml:space="preserve">liter</t>
@@ -69,7 +69,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -97,12 +97,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -173,53 +167,53 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z65536"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -550,7 +544,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
BB-21713: Optimize Quick Order Form (#34141)
</commit_message>
<xml_diff>
--- a/src/Oro/Bundle/ProductBundle/Tests/Functional/Controller/Frontend/files/quick-order.xlsx
+++ b/src/Oro/Bundle/ProductBundle/Tests/Functional/Controller/Frontend/files/quick-order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">product-1</t>
   </si>
   <si>
-    <t xml:space="preserve">1,4</t>
+    <t xml:space="preserve">1.4</t>
   </si>
   <si>
     <t xml:space="preserve">liter</t>
@@ -69,7 +69,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -97,12 +97,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -173,53 +167,53 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z65536"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -550,7 +544,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
BB-22738: Product Kits in Quick Order Form (#37614)
* BB-23583: [Backend] Ensure product kit can be added to Quick Order Form (#37540)

- enabled Product Kits for Quick Order Form;
- added hide price for Product Kit rows;
- added field "type" to the QuickAddModel;
- set QuickAddRow::type value through BasicQuickAddCollectionNormalizer;
- fixed a problem with a missed relation to the "doctrine" service in some controllers

* BB-23585: [Backend] Ensure Create Order button works on QOF with kit line items (#37590)

- disabled "Create Order" button if Quick Order Form has Product Kits;
- added a title attribute to "Create Order" button

* BB-23587: [Backend] Behat tests (#37609)
</commit_message>
<xml_diff>
--- a/src/Oro/Bundle/ProductBundle/Tests/Functional/Controller/Frontend/files/quick-order.xlsx
+++ b/src/Oro/Bundle/ProductBundle/Tests/Functional/Controller/Frontend/files/quick-order.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t xml:space="preserve">Item Number</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t xml:space="preserve">SKU3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product-kit-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">milliliter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product-kit-2</t>
   </si>
 </sst>
 </file>
@@ -207,13 +216,13 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -540,11 +549,46 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>